<commit_message>
Agregando diferencias relativas y normalizadas para el analisis
</commit_message>
<xml_diff>
--- a/Datos/Bases JASP/Reset_Ttest.xlsx
+++ b/Datos/Bases JASP/Reset_Ttest.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="43">
   <si>
     <t>Sesion</t>
   </si>
@@ -81,6 +81,78 @@
   </si>
   <si>
     <t>Choice_5</t>
+  </si>
+  <si>
+    <t>aDO1_4</t>
+  </si>
+  <si>
+    <t>aDO1_5</t>
+  </si>
+  <si>
+    <t>aDOP_4</t>
+  </si>
+  <si>
+    <t>aDOP_5</t>
+  </si>
+  <si>
+    <t>aDA_4</t>
+  </si>
+  <si>
+    <t>aDA_5</t>
+  </si>
+  <si>
+    <t>aDAP_4</t>
+  </si>
+  <si>
+    <t>aDAP_5</t>
+  </si>
+  <si>
+    <t>rDO1_4</t>
+  </si>
+  <si>
+    <t>rDO1_5</t>
+  </si>
+  <si>
+    <t>rDOP_4</t>
+  </si>
+  <si>
+    <t>rDOP_5</t>
+  </si>
+  <si>
+    <t>rDA_4</t>
+  </si>
+  <si>
+    <t>rDA_5</t>
+  </si>
+  <si>
+    <t>rDAP_4</t>
+  </si>
+  <si>
+    <t>rDAP_5</t>
+  </si>
+  <si>
+    <t>nDO1_4</t>
+  </si>
+  <si>
+    <t>nDO1_5</t>
+  </si>
+  <si>
+    <t>nDOP_4</t>
+  </si>
+  <si>
+    <t>nDOP_5</t>
+  </si>
+  <si>
+    <t>nDA_4</t>
+  </si>
+  <si>
+    <t>nDA_5</t>
+  </si>
+  <si>
+    <t>nDAP_4</t>
+  </si>
+  <si>
+    <t>nDAP_5</t>
   </si>
 </sst>
 </file>
@@ -96,12 +168,48 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -116,8 +224,14 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -398,664 +512,1549 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:S11"/>
+  <dimension ref="A1:AQ11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+    <sheetView tabSelected="1" topLeftCell="J1" workbookViewId="0">
+      <selection activeCell="AQ12" sqref="AQ12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="3" width="11.42578125" style="2"/>
+    <col min="4" max="11" width="11.42578125" style="4"/>
+    <col min="12" max="12" width="6.85546875" style="5" customWidth="1"/>
+    <col min="13" max="13" width="7.42578125" style="5" customWidth="1"/>
+    <col min="14" max="14" width="11.42578125" style="5" customWidth="1"/>
+    <col min="15" max="19" width="11.42578125" style="5"/>
+    <col min="20" max="20" width="11.85546875" style="6" bestFit="1" customWidth="1"/>
+    <col min="21" max="27" width="11.42578125" style="6"/>
+    <col min="28" max="35" width="11.42578125" style="3"/>
+    <col min="36" max="43" width="11.42578125" style="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="E1" t="s">
+      <c r="E1" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="F1" t="s">
+      <c r="F1" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="G1" t="s">
+      <c r="G1" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="H1" t="s">
+      <c r="H1" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="I1" t="s">
+      <c r="I1" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="J1" t="s">
+      <c r="J1" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="K1" t="s">
+      <c r="K1" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="L1" t="s">
+      <c r="L1" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="M1" t="s">
+      <c r="M1" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="N1" t="s">
+      <c r="N1" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="O1" t="s">
+      <c r="O1" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="P1" t="s">
+      <c r="P1" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="Q1" t="s">
+      <c r="Q1" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="R1" t="s">
+      <c r="R1" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="S1" t="s">
+      <c r="S1" s="5" t="s">
         <v>16</v>
       </c>
+      <c r="T1" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="U1" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="V1" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="W1" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="X1" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="Y1" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="Z1" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="AA1" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="AB1" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="AC1" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="AD1" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="AE1" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="AF1" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="AG1" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="AH1" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="AI1" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="AJ1" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="AK1" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="AL1" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="AM1" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="AN1" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="AO1" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="AP1" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="AQ1" s="1" t="s">
+        <v>42</v>
+      </c>
     </row>
-    <row r="2" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
-      <c r="B2">
+      <c r="B2" s="2">
         <v>7</v>
       </c>
-      <c r="C2">
+      <c r="C2" s="2">
         <v>23</v>
       </c>
-      <c r="D2">
+      <c r="D2" s="4">
         <v>25</v>
       </c>
-      <c r="E2">
+      <c r="E2" s="4">
         <v>40</v>
       </c>
-      <c r="F2">
+      <c r="F2" s="4">
         <v>16.66667</v>
       </c>
-      <c r="G2">
+      <c r="G2" s="4">
         <v>26.66667</v>
       </c>
-      <c r="H2">
+      <c r="H2" s="4">
         <v>19</v>
       </c>
-      <c r="I2">
+      <c r="I2" s="4">
         <v>34.333300000000001</v>
       </c>
-      <c r="J2">
+      <c r="J2" s="4">
         <v>12.66667</v>
       </c>
-      <c r="K2">
+      <c r="K2" s="4">
         <v>22.88889</v>
       </c>
-      <c r="L2">
+      <c r="L2" s="5">
         <v>18</v>
       </c>
-      <c r="M2">
+      <c r="M2" s="5">
         <v>17</v>
       </c>
-      <c r="N2">
+      <c r="N2" s="5">
         <v>9.6666600000000003</v>
       </c>
-      <c r="O2">
+      <c r="O2" s="5">
         <v>3.6666599999999998</v>
       </c>
-      <c r="P2">
+      <c r="P2" s="5">
         <v>12</v>
       </c>
-      <c r="Q2">
+      <c r="Q2" s="5">
         <v>11.33333</v>
       </c>
-      <c r="R2">
+      <c r="R2" s="5">
         <v>5.6666600000000003</v>
       </c>
-      <c r="S2">
+      <c r="S2" s="5">
         <v>-0.111111</v>
       </c>
+      <c r="T2" s="6">
+        <f>ABS(L2)</f>
+        <v>18</v>
+      </c>
+      <c r="U2" s="6">
+        <f t="shared" ref="U2:AA11" si="0">ABS(M2)</f>
+        <v>17</v>
+      </c>
+      <c r="V2" s="6">
+        <f t="shared" si="0"/>
+        <v>9.6666600000000003</v>
+      </c>
+      <c r="W2" s="6">
+        <f t="shared" si="0"/>
+        <v>3.6666599999999998</v>
+      </c>
+      <c r="X2" s="6">
+        <f t="shared" si="0"/>
+        <v>12</v>
+      </c>
+      <c r="Y2" s="6">
+        <f t="shared" si="0"/>
+        <v>11.33333</v>
+      </c>
+      <c r="Z2" s="6">
+        <f t="shared" si="0"/>
+        <v>5.6666600000000003</v>
+      </c>
+      <c r="AA2" s="6">
+        <f t="shared" si="0"/>
+        <v>0.111111</v>
+      </c>
+      <c r="AB2" s="3">
+        <v>-1.125</v>
+      </c>
+      <c r="AC2" s="3">
+        <v>-0.54</v>
+      </c>
+      <c r="AD2" s="3">
+        <v>-0.81699999999999995</v>
+      </c>
+      <c r="AE2" s="3">
+        <v>-0.14799999999999999</v>
+      </c>
+      <c r="AF2" s="3">
+        <v>-0.92300000000000004</v>
+      </c>
+      <c r="AG2" s="3">
+        <v>-0.39500000000000002</v>
+      </c>
+      <c r="AH2" s="3">
+        <v>-0.57599999999999996</v>
+      </c>
+      <c r="AI2" s="3">
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="AJ2" s="1">
+        <v>1.4590000000000001</v>
+      </c>
+      <c r="AK2" s="1">
+        <v>0.30499999999999999</v>
+      </c>
+      <c r="AL2" s="1">
+        <v>0.78400000000000003</v>
+      </c>
+      <c r="AM2" s="1">
+        <v>6.6000000000000003E-2</v>
+      </c>
+      <c r="AN2" s="1">
+        <v>0.97299999999999998</v>
+      </c>
+      <c r="AO2" s="1">
+        <v>0.20399999999999999</v>
+      </c>
+      <c r="AP2" s="1">
+        <v>0.45900000000000002</v>
+      </c>
+      <c r="AQ2" s="1">
+        <v>-2E-3</v>
+      </c>
     </row>
-    <row r="3" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
-      <c r="B3">
+      <c r="B3" s="2">
         <v>28</v>
       </c>
-      <c r="C3">
+      <c r="C3" s="2">
         <v>25</v>
       </c>
-      <c r="D3">
+      <c r="D3" s="4">
         <v>34</v>
       </c>
-      <c r="E3">
+      <c r="E3" s="4">
         <v>40</v>
       </c>
-      <c r="F3">
+      <c r="F3" s="4">
         <v>22.66667</v>
       </c>
-      <c r="G3">
+      <c r="G3" s="4">
         <v>26.66667</v>
       </c>
-      <c r="H3">
+      <c r="H3" s="4">
         <v>32</v>
       </c>
-      <c r="I3">
+      <c r="I3" s="4">
         <v>35</v>
       </c>
-      <c r="J3">
+      <c r="J3" s="4">
         <v>21.33333</v>
       </c>
-      <c r="K3">
+      <c r="K3" s="4">
         <v>23.33333</v>
       </c>
-      <c r="L3">
+      <c r="L3" s="5">
         <v>6</v>
       </c>
-      <c r="M3">
+      <c r="M3" s="5">
         <v>15</v>
       </c>
-      <c r="N3">
+      <c r="N3" s="5">
         <v>-5.3333300000000001</v>
       </c>
-      <c r="O3">
+      <c r="O3" s="5">
         <v>1.6666669999999999</v>
       </c>
-      <c r="P3">
+      <c r="P3" s="5">
         <v>4</v>
       </c>
-      <c r="Q3">
+      <c r="Q3" s="5">
         <v>10</v>
       </c>
-      <c r="R3">
+      <c r="R3" s="5">
         <v>-6.6665999999999999</v>
       </c>
-      <c r="S3">
+      <c r="S3" s="5">
         <v>-1.66666</v>
       </c>
+      <c r="T3" s="6">
+        <f t="shared" ref="T3:T11" si="1">ABS(L3)</f>
+        <v>6</v>
+      </c>
+      <c r="U3" s="6">
+        <f t="shared" si="0"/>
+        <v>15</v>
+      </c>
+      <c r="V3" s="6">
+        <f t="shared" si="0"/>
+        <v>5.3333300000000001</v>
+      </c>
+      <c r="W3" s="6">
+        <f t="shared" si="0"/>
+        <v>1.6666669999999999</v>
+      </c>
+      <c r="X3" s="6">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+      <c r="Y3" s="6">
+        <f t="shared" si="0"/>
+        <v>10</v>
+      </c>
+      <c r="Z3" s="6">
+        <f t="shared" si="0"/>
+        <v>6.6665999999999999</v>
+      </c>
+      <c r="AA3" s="6">
+        <f t="shared" si="0"/>
+        <v>1.66666</v>
+      </c>
+      <c r="AB3" s="3">
+        <v>-0.19400000000000001</v>
+      </c>
+      <c r="AC3" s="3">
+        <v>-0.46200000000000002</v>
+      </c>
+      <c r="AD3" s="3">
+        <v>0.21099999999999999</v>
+      </c>
+      <c r="AE3" s="3">
+        <v>-6.5000000000000002E-2</v>
+      </c>
+      <c r="AF3" s="3">
+        <v>-0.13300000000000001</v>
+      </c>
+      <c r="AG3" s="3">
+        <v>-0.33300000000000002</v>
+      </c>
+      <c r="AH3" s="3">
+        <v>0.27</v>
+      </c>
+      <c r="AI3" s="3">
+        <v>6.9000000000000006E-2</v>
+      </c>
+      <c r="AJ3" s="1">
+        <v>0.19400000000000001</v>
+      </c>
+      <c r="AK3" s="1">
+        <v>0.23</v>
+      </c>
+      <c r="AL3" s="1">
+        <v>-0.17199999999999999</v>
+      </c>
+      <c r="AM3" s="1">
+        <v>2.5999999999999999E-2</v>
+      </c>
+      <c r="AN3" s="1">
+        <v>0.129</v>
+      </c>
+      <c r="AO3" s="1">
+        <v>0.153</v>
+      </c>
+      <c r="AP3" s="1">
+        <v>-0.215</v>
+      </c>
+      <c r="AQ3" s="1">
+        <v>-2.5999999999999999E-2</v>
+      </c>
     </row>
-    <row r="4" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>3</v>
       </c>
-      <c r="B4">
+      <c r="B4" s="2">
         <v>81</v>
       </c>
-      <c r="C4">
+      <c r="C4" s="2">
         <v>16</v>
       </c>
-      <c r="D4">
+      <c r="D4" s="4">
         <v>65.5</v>
       </c>
-      <c r="E4">
+      <c r="E4" s="4">
         <v>32</v>
       </c>
-      <c r="F4">
+      <c r="F4" s="4">
         <v>43.666699999999999</v>
       </c>
-      <c r="G4">
+      <c r="G4" s="4">
         <v>21.333300000000001</v>
       </c>
-      <c r="H4">
+      <c r="H4" s="4">
         <v>70.666669999999996</v>
       </c>
-      <c r="I4">
+      <c r="I4" s="4">
         <v>26.66667</v>
       </c>
-      <c r="J4">
+      <c r="J4" s="4">
         <v>47.111109999999996</v>
       </c>
-      <c r="K4">
+      <c r="K4" s="4">
         <v>17.77778</v>
       </c>
-      <c r="L4">
+      <c r="L4" s="5">
         <v>-15.5</v>
       </c>
-      <c r="M4">
+      <c r="M4" s="5">
         <v>16</v>
       </c>
-      <c r="N4">
+      <c r="N4" s="5">
         <v>-37.333329999999997</v>
       </c>
-      <c r="O4">
+      <c r="O4" s="5">
         <v>5.3333300000000001</v>
       </c>
-      <c r="P4">
+      <c r="P4" s="5">
         <v>-10.33333</v>
       </c>
-      <c r="Q4">
+      <c r="Q4" s="5">
         <v>10.66667</v>
       </c>
-      <c r="R4">
+      <c r="R4" s="5">
         <v>-33.88888</v>
       </c>
-      <c r="S4">
+      <c r="S4" s="5">
         <v>1.7777700000000001</v>
       </c>
+      <c r="T4" s="6">
+        <f t="shared" si="1"/>
+        <v>15.5</v>
+      </c>
+      <c r="U4" s="6">
+        <f t="shared" si="0"/>
+        <v>16</v>
+      </c>
+      <c r="V4" s="6">
+        <f t="shared" si="0"/>
+        <v>37.333329999999997</v>
+      </c>
+      <c r="W4" s="6">
+        <f t="shared" si="0"/>
+        <v>5.3333300000000001</v>
+      </c>
+      <c r="X4" s="6">
+        <f t="shared" si="0"/>
+        <v>10.33333</v>
+      </c>
+      <c r="Y4" s="6">
+        <f t="shared" si="0"/>
+        <v>10.66667</v>
+      </c>
+      <c r="Z4" s="6">
+        <f t="shared" si="0"/>
+        <v>33.88888</v>
+      </c>
+      <c r="AA4" s="6">
+        <f t="shared" si="0"/>
+        <v>1.7777700000000001</v>
+      </c>
+      <c r="AB4" s="3">
+        <v>0.21199999999999999</v>
+      </c>
+      <c r="AC4" s="3">
+        <v>-0.66700000000000004</v>
+      </c>
+      <c r="AD4" s="3">
+        <v>0.59899999999999998</v>
+      </c>
+      <c r="AE4" s="3">
+        <v>-0.28599999999999998</v>
+      </c>
+      <c r="AF4" s="3">
+        <v>0.13600000000000001</v>
+      </c>
+      <c r="AG4" s="3">
+        <v>-0.5</v>
+      </c>
+      <c r="AH4" s="3">
+        <v>0.52900000000000003</v>
+      </c>
+      <c r="AI4" s="3">
+        <v>-0.105</v>
+      </c>
+      <c r="AJ4" s="1">
+        <v>-0.27700000000000002</v>
+      </c>
+      <c r="AK4" s="1">
+        <v>0.58499999999999996</v>
+      </c>
+      <c r="AL4" s="1">
+        <v>-0.66700000000000004</v>
+      </c>
+      <c r="AM4" s="1">
+        <v>0.19500000000000001</v>
+      </c>
+      <c r="AN4" s="1">
+        <v>-0.185</v>
+      </c>
+      <c r="AO4" s="1">
+        <v>0.39</v>
+      </c>
+      <c r="AP4" s="1">
+        <v>-0.60499999999999998</v>
+      </c>
+      <c r="AQ4" s="1">
+        <v>6.5000000000000002E-2</v>
+      </c>
     </row>
-    <row r="5" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>4</v>
       </c>
-      <c r="B5">
+      <c r="B5" s="2">
         <v>14</v>
       </c>
-      <c r="C5">
+      <c r="C5" s="2">
         <v>15</v>
       </c>
-      <c r="D5">
+      <c r="D5" s="4">
         <v>18</v>
       </c>
-      <c r="E5">
+      <c r="E5" s="4">
         <v>13</v>
       </c>
-      <c r="F5">
+      <c r="F5" s="4">
         <v>12</v>
       </c>
-      <c r="G5">
+      <c r="G5" s="4">
         <v>8.6666000000000007</v>
       </c>
-      <c r="H5">
+      <c r="H5" s="4">
         <v>16.66667</v>
       </c>
-      <c r="I5">
+      <c r="I5" s="4">
         <v>13.66667</v>
       </c>
-      <c r="J5">
+      <c r="J5" s="4">
         <v>11.11111</v>
       </c>
-      <c r="K5">
+      <c r="K5" s="4">
         <v>9.11111</v>
       </c>
-      <c r="L5">
+      <c r="L5" s="5">
         <v>4</v>
       </c>
-      <c r="M5">
+      <c r="M5" s="5">
         <v>-2</v>
       </c>
-      <c r="N5">
+      <c r="N5" s="5">
         <v>-2</v>
       </c>
-      <c r="O5">
+      <c r="O5" s="5">
         <v>-6.3333300000000001</v>
       </c>
-      <c r="P5">
+      <c r="P5" s="5">
         <v>2.6666599999999998</v>
       </c>
-      <c r="Q5">
+      <c r="Q5" s="5">
         <v>-1.3332999999999999</v>
       </c>
-      <c r="R5">
+      <c r="R5" s="5">
         <v>-2.8888880000000001</v>
       </c>
-      <c r="S5">
+      <c r="S5" s="5">
         <v>-5.8888800000000003</v>
       </c>
+      <c r="T5" s="6">
+        <f t="shared" si="1"/>
+        <v>4</v>
+      </c>
+      <c r="U5" s="6">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="V5" s="6">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="W5" s="6">
+        <f t="shared" si="0"/>
+        <v>6.3333300000000001</v>
+      </c>
+      <c r="X5" s="6">
+        <f t="shared" si="0"/>
+        <v>2.6666599999999998</v>
+      </c>
+      <c r="Y5" s="6">
+        <f t="shared" si="0"/>
+        <v>1.3332999999999999</v>
+      </c>
+      <c r="Z5" s="6">
+        <f t="shared" si="0"/>
+        <v>2.8888880000000001</v>
+      </c>
+      <c r="AA5" s="6">
+        <f t="shared" si="0"/>
+        <v>5.8888800000000003</v>
+      </c>
+      <c r="AB5" s="3">
+        <v>-0.25</v>
+      </c>
+      <c r="AC5" s="3">
+        <v>0.14299999999999999</v>
+      </c>
+      <c r="AD5" s="3">
+        <v>0.154</v>
+      </c>
+      <c r="AE5" s="3">
+        <v>0.53500000000000003</v>
+      </c>
+      <c r="AF5" s="3">
+        <v>-0.17399999999999999</v>
+      </c>
+      <c r="AG5" s="3">
+        <v>9.2999999999999999E-2</v>
+      </c>
+      <c r="AH5" s="3">
+        <v>0.23</v>
+      </c>
+      <c r="AI5" s="3">
+        <v>0.48799999999999999</v>
+      </c>
+      <c r="AJ5" s="1">
+        <v>0.23100000000000001</v>
+      </c>
+      <c r="AK5" s="1">
+        <v>-8.5999999999999993E-2</v>
+      </c>
+      <c r="AL5" s="1">
+        <v>-0.115</v>
+      </c>
+      <c r="AM5" s="1">
+        <v>-0.27100000000000002</v>
+      </c>
+      <c r="AN5" s="1">
+        <v>0.154</v>
+      </c>
+      <c r="AO5" s="1">
+        <v>-5.7000000000000002E-2</v>
+      </c>
+      <c r="AP5" s="1">
+        <v>-0.16700000000000001</v>
+      </c>
+      <c r="AQ5" s="1">
+        <v>-0.252</v>
+      </c>
     </row>
-    <row r="6" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>5</v>
       </c>
-      <c r="B6">
+      <c r="B6" s="2">
         <v>3</v>
       </c>
-      <c r="C6">
+      <c r="C6" s="2">
         <v>22</v>
       </c>
-      <c r="D6">
+      <c r="D6" s="4">
         <v>11</v>
       </c>
-      <c r="E6">
+      <c r="E6" s="4">
         <v>67.5</v>
       </c>
-      <c r="F6">
+      <c r="F6" s="4">
         <v>7.3333000000000004</v>
       </c>
-      <c r="G6">
+      <c r="G6" s="4">
         <v>45</v>
       </c>
-      <c r="H6">
+      <c r="H6" s="4">
         <v>8.3332999999999995</v>
       </c>
-      <c r="I6">
+      <c r="I6" s="4">
         <v>52.333300000000001</v>
       </c>
-      <c r="J6">
+      <c r="J6" s="4">
         <v>5.5555500000000002</v>
       </c>
-      <c r="K6">
+      <c r="K6" s="4">
         <v>34.88888</v>
       </c>
-      <c r="L6">
+      <c r="L6" s="5">
         <v>8</v>
       </c>
-      <c r="M6">
+      <c r="M6" s="5">
         <v>45.5</v>
       </c>
-      <c r="N6">
+      <c r="N6" s="5">
         <v>4.3333300000000001</v>
       </c>
-      <c r="O6">
+      <c r="O6" s="5">
         <v>23</v>
       </c>
-      <c r="P6">
+      <c r="P6" s="5">
         <v>5.3333000000000004</v>
       </c>
-      <c r="Q6">
+      <c r="Q6" s="5">
         <v>30.33333</v>
       </c>
-      <c r="R6">
+      <c r="R6" s="5">
         <v>2.555555</v>
       </c>
-      <c r="S6">
+      <c r="S6" s="5">
         <v>12.88888</v>
       </c>
+      <c r="T6" s="6">
+        <f t="shared" si="1"/>
+        <v>8</v>
+      </c>
+      <c r="U6" s="6">
+        <f t="shared" si="0"/>
+        <v>45.5</v>
+      </c>
+      <c r="V6" s="6">
+        <f t="shared" si="0"/>
+        <v>4.3333300000000001</v>
+      </c>
+      <c r="W6" s="6">
+        <f t="shared" si="0"/>
+        <v>23</v>
+      </c>
+      <c r="X6" s="6">
+        <f t="shared" si="0"/>
+        <v>5.3333000000000004</v>
+      </c>
+      <c r="Y6" s="6">
+        <f t="shared" si="0"/>
+        <v>30.33333</v>
+      </c>
+      <c r="Z6" s="6">
+        <f t="shared" si="0"/>
+        <v>2.555555</v>
+      </c>
+      <c r="AA6" s="6">
+        <f t="shared" si="0"/>
+        <v>12.88888</v>
+      </c>
+      <c r="AB6" s="3">
+        <v>-1.143</v>
+      </c>
+      <c r="AC6" s="3">
+        <v>-1.0169999999999999</v>
+      </c>
+      <c r="AD6" s="3">
+        <v>-0.83899999999999997</v>
+      </c>
+      <c r="AE6" s="3">
+        <v>-0.68700000000000006</v>
+      </c>
+      <c r="AF6" s="3">
+        <v>-0.94099999999999995</v>
+      </c>
+      <c r="AG6" s="3">
+        <v>-0.81599999999999995</v>
+      </c>
+      <c r="AH6" s="3">
+        <v>-0.59699999999999998</v>
+      </c>
+      <c r="AI6" s="3">
+        <v>-0.45300000000000001</v>
+      </c>
+      <c r="AJ6" s="1">
+        <v>1.091</v>
+      </c>
+      <c r="AK6" s="1">
+        <v>1.4370000000000001</v>
+      </c>
+      <c r="AL6" s="1">
+        <v>0.59099999999999997</v>
+      </c>
+      <c r="AM6" s="1">
+        <v>0.72599999999999998</v>
+      </c>
+      <c r="AN6" s="1">
+        <v>0.72699999999999998</v>
+      </c>
+      <c r="AO6" s="1">
+        <v>0.95799999999999996</v>
+      </c>
+      <c r="AP6" s="1">
+        <v>0.34799999999999998</v>
+      </c>
+      <c r="AQ6" s="1">
+        <v>0.40699999999999997</v>
+      </c>
     </row>
-    <row r="7" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>6</v>
       </c>
-      <c r="B7">
+      <c r="B7" s="2">
         <v>23</v>
       </c>
-      <c r="C7">
+      <c r="C7" s="2">
         <v>13</v>
       </c>
-      <c r="D7">
+      <c r="D7" s="4">
         <v>16</v>
       </c>
-      <c r="E7">
+      <c r="E7" s="4">
         <v>23</v>
       </c>
-      <c r="F7">
+      <c r="F7" s="4">
         <v>10.66667</v>
       </c>
-      <c r="G7">
+      <c r="G7" s="4">
         <v>15.333299999999999</v>
       </c>
-      <c r="H7">
+      <c r="H7" s="4">
         <v>18.333300000000001</v>
       </c>
-      <c r="I7">
+      <c r="I7" s="4">
         <v>19.66667</v>
       </c>
-      <c r="J7">
+      <c r="J7" s="4">
         <v>12.22222</v>
       </c>
-      <c r="K7">
+      <c r="K7" s="4">
         <v>13.11111</v>
       </c>
-      <c r="L7">
+      <c r="L7" s="5">
         <v>-7</v>
       </c>
-      <c r="M7">
+      <c r="M7" s="5">
         <v>10</v>
       </c>
-      <c r="N7">
+      <c r="N7" s="5">
         <v>-12.33333</v>
       </c>
-      <c r="O7">
+      <c r="O7" s="5">
         <v>2.3333330000000001</v>
       </c>
-      <c r="P7">
+      <c r="P7" s="5">
         <v>-4.6666699999999999</v>
       </c>
-      <c r="Q7">
+      <c r="Q7" s="5">
         <v>6.6666600000000003</v>
       </c>
-      <c r="R7">
+      <c r="R7" s="5">
         <v>-10.77777</v>
       </c>
-      <c r="S7">
+      <c r="S7" s="5">
         <v>0.111111</v>
       </c>
+      <c r="T7" s="6">
+        <f t="shared" si="1"/>
+        <v>7</v>
+      </c>
+      <c r="U7" s="6">
+        <f t="shared" si="0"/>
+        <v>10</v>
+      </c>
+      <c r="V7" s="6">
+        <f t="shared" si="0"/>
+        <v>12.33333</v>
+      </c>
+      <c r="W7" s="6">
+        <f t="shared" si="0"/>
+        <v>2.3333330000000001</v>
+      </c>
+      <c r="X7" s="6">
+        <f t="shared" si="0"/>
+        <v>4.6666699999999999</v>
+      </c>
+      <c r="Y7" s="6">
+        <f t="shared" si="0"/>
+        <v>6.6666600000000003</v>
+      </c>
+      <c r="Z7" s="6">
+        <f t="shared" si="0"/>
+        <v>10.77777</v>
+      </c>
+      <c r="AA7" s="6">
+        <f t="shared" si="0"/>
+        <v>0.111111</v>
+      </c>
+      <c r="AB7" s="3">
+        <v>0.35899999999999999</v>
+      </c>
+      <c r="AC7" s="3">
+        <v>-0.55600000000000005</v>
+      </c>
+      <c r="AD7" s="3">
+        <v>0.73299999999999998</v>
+      </c>
+      <c r="AE7" s="3">
+        <v>-0.16500000000000001</v>
+      </c>
+      <c r="AF7" s="3">
+        <v>0.22600000000000001</v>
+      </c>
+      <c r="AG7" s="3">
+        <v>-0.40799999999999997</v>
+      </c>
+      <c r="AH7" s="3">
+        <v>0.61199999999999999</v>
+      </c>
+      <c r="AI7" s="3">
+        <v>-8.9999999999999993E-3</v>
+      </c>
+      <c r="AJ7" s="1">
+        <v>-0.3</v>
+      </c>
+      <c r="AK7" s="1">
+        <v>0.47599999999999998</v>
+      </c>
+      <c r="AL7" s="1">
+        <v>-0.52900000000000003</v>
+      </c>
+      <c r="AM7" s="1">
+        <v>0.111</v>
+      </c>
+      <c r="AN7" s="1">
+        <v>-0.2</v>
+      </c>
+      <c r="AO7" s="1">
+        <v>0.317</v>
+      </c>
+      <c r="AP7" s="1">
+        <v>-0.46200000000000002</v>
+      </c>
+      <c r="AQ7" s="1">
+        <v>5.0000000000000001E-3</v>
+      </c>
     </row>
-    <row r="8" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>7</v>
       </c>
-      <c r="B8">
+      <c r="B8" s="2">
         <v>15</v>
       </c>
-      <c r="C8">
+      <c r="C8" s="2">
         <v>28</v>
       </c>
-      <c r="D8">
+      <c r="D8" s="4">
         <v>20.5</v>
       </c>
-      <c r="E8">
+      <c r="E8" s="4">
         <v>41</v>
       </c>
-      <c r="F8">
+      <c r="F8" s="4">
         <v>13.66667</v>
       </c>
-      <c r="G8">
+      <c r="G8" s="4">
         <v>27.333300000000001</v>
       </c>
-      <c r="H8">
+      <c r="H8" s="4">
         <v>18.66667</v>
       </c>
-      <c r="I8">
+      <c r="I8" s="4">
         <v>36.666670000000003</v>
       </c>
-      <c r="J8">
+      <c r="J8" s="4">
         <v>12.44444</v>
       </c>
-      <c r="K8">
+      <c r="K8" s="4">
         <v>24.44444</v>
       </c>
-      <c r="L8">
+      <c r="L8" s="5">
         <v>5.5</v>
       </c>
-      <c r="M8">
+      <c r="M8" s="5">
         <v>13</v>
       </c>
-      <c r="N8">
+      <c r="N8" s="5">
         <v>-1.3333299999999999</v>
       </c>
-      <c r="O8">
+      <c r="O8" s="5">
         <v>-0.66666599999999998</v>
       </c>
-      <c r="P8">
+      <c r="P8" s="5">
         <v>3.6666599999999998</v>
       </c>
-      <c r="Q8">
+      <c r="Q8" s="5">
         <v>8.6666659999999993</v>
       </c>
-      <c r="R8">
+      <c r="R8" s="5">
         <v>-2.555555</v>
       </c>
-      <c r="S8">
+      <c r="S8" s="5">
         <v>-3.5555500000000002</v>
       </c>
+      <c r="T8" s="6">
+        <f t="shared" si="1"/>
+        <v>5.5</v>
+      </c>
+      <c r="U8" s="6">
+        <f t="shared" si="0"/>
+        <v>13</v>
+      </c>
+      <c r="V8" s="6">
+        <f t="shared" si="0"/>
+        <v>1.3333299999999999</v>
+      </c>
+      <c r="W8" s="6">
+        <f t="shared" si="0"/>
+        <v>0.66666599999999998</v>
+      </c>
+      <c r="X8" s="6">
+        <f t="shared" si="0"/>
+        <v>3.6666599999999998</v>
+      </c>
+      <c r="Y8" s="6">
+        <f t="shared" si="0"/>
+        <v>8.6666659999999993</v>
+      </c>
+      <c r="Z8" s="6">
+        <f t="shared" si="0"/>
+        <v>2.555555</v>
+      </c>
+      <c r="AA8" s="6">
+        <f t="shared" si="0"/>
+        <v>3.5555500000000002</v>
+      </c>
+      <c r="AB8" s="3">
+        <v>-0.31</v>
+      </c>
+      <c r="AC8" s="3">
+        <v>-0.377</v>
+      </c>
+      <c r="AD8" s="3">
+        <v>9.2999999999999999E-2</v>
+      </c>
+      <c r="AE8" s="3">
+        <v>2.4E-2</v>
+      </c>
+      <c r="AF8" s="3">
+        <v>-0.218</v>
+      </c>
+      <c r="AG8" s="3">
+        <v>-0.26800000000000002</v>
+      </c>
+      <c r="AH8" s="3">
+        <v>0.186</v>
+      </c>
+      <c r="AI8" s="3">
+        <v>-136</v>
+      </c>
+      <c r="AJ8" s="1">
+        <v>0.154</v>
+      </c>
+      <c r="AK8" s="1">
+        <v>0.36799999999999999</v>
+      </c>
+      <c r="AL8" s="1">
+        <v>-3.6999999999999998E-2</v>
+      </c>
+      <c r="AM8" s="1">
+        <v>-1.9E-2</v>
+      </c>
+      <c r="AN8" s="1">
+        <v>0.10299999999999999</v>
+      </c>
+      <c r="AO8" s="1">
+        <v>0.245</v>
+      </c>
+      <c r="AP8" s="1">
+        <v>-7.1999999999999995E-2</v>
+      </c>
+      <c r="AQ8" s="1">
+        <v>-0.10100000000000001</v>
+      </c>
     </row>
-    <row r="9" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>8</v>
       </c>
-      <c r="B9">
+      <c r="B9" s="2">
         <v>25</v>
       </c>
-      <c r="C9">
+      <c r="C9" s="2">
         <v>40</v>
       </c>
-      <c r="D9">
+      <c r="D9" s="4">
         <v>25</v>
       </c>
-      <c r="E9">
+      <c r="E9" s="4">
         <v>40</v>
       </c>
-      <c r="F9">
+      <c r="F9" s="4">
         <v>16.666699999999999</v>
       </c>
-      <c r="G9">
+      <c r="G9" s="4">
         <v>26.66667</v>
       </c>
-      <c r="H9">
+      <c r="H9" s="4">
         <v>25</v>
       </c>
-      <c r="I9">
+      <c r="I9" s="4">
         <v>40</v>
       </c>
-      <c r="J9">
+      <c r="J9" s="4">
         <v>16.66667</v>
       </c>
-      <c r="K9">
+      <c r="K9" s="4">
         <v>26.66667</v>
       </c>
-      <c r="L9">
-        <v>0</v>
-      </c>
-      <c r="M9">
-        <v>0</v>
-      </c>
-      <c r="N9">
+      <c r="L9" s="5">
+        <v>0</v>
+      </c>
+      <c r="M9" s="5">
+        <v>0</v>
+      </c>
+      <c r="N9" s="5">
         <v>-8.3333329999999997</v>
       </c>
-      <c r="O9">
+      <c r="O9" s="5">
         <v>-13.33333</v>
       </c>
-      <c r="P9">
-        <v>0</v>
-      </c>
-      <c r="Q9">
-        <v>0</v>
-      </c>
-      <c r="R9">
+      <c r="P9" s="5">
+        <v>0</v>
+      </c>
+      <c r="Q9" s="5">
+        <v>0</v>
+      </c>
+      <c r="R9" s="5">
         <v>-8.3333300000000001</v>
       </c>
-      <c r="S9">
+      <c r="S9" s="5">
         <v>-13.33333</v>
       </c>
+      <c r="T9" s="6">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="U9" s="6">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="V9" s="6">
+        <f t="shared" si="0"/>
+        <v>8.3333329999999997</v>
+      </c>
+      <c r="W9" s="6">
+        <f t="shared" si="0"/>
+        <v>13.33333</v>
+      </c>
+      <c r="X9" s="6">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="Y9" s="6">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="Z9" s="6">
+        <f t="shared" si="0"/>
+        <v>8.3333300000000001</v>
+      </c>
+      <c r="AA9" s="6">
+        <f t="shared" si="0"/>
+        <v>13.33333</v>
+      </c>
+      <c r="AB9" s="3">
+        <v>0</v>
+      </c>
+      <c r="AC9" s="3">
+        <v>0</v>
+      </c>
+      <c r="AD9" s="3">
+        <v>0.4</v>
+      </c>
+      <c r="AE9" s="3">
+        <v>0.4</v>
+      </c>
+      <c r="AF9" s="3">
+        <v>0</v>
+      </c>
+      <c r="AG9" s="3">
+        <v>0</v>
+      </c>
+      <c r="AH9" s="3">
+        <v>0.4</v>
+      </c>
+      <c r="AI9" s="3">
+        <v>0.4</v>
+      </c>
+      <c r="AJ9" s="1">
+        <v>0</v>
+      </c>
+      <c r="AK9" s="1">
+        <v>0</v>
+      </c>
+      <c r="AL9" s="1">
+        <v>-0.30499999999999999</v>
+      </c>
+      <c r="AM9" s="1">
+        <v>-0.48799999999999999</v>
+      </c>
+      <c r="AN9" s="1">
+        <v>0</v>
+      </c>
+      <c r="AO9" s="1">
+        <v>0</v>
+      </c>
+      <c r="AP9" s="1">
+        <v>-0.30499999999999999</v>
+      </c>
+      <c r="AQ9" s="1">
+        <v>-0.48799999999999999</v>
+      </c>
     </row>
-    <row r="10" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>9</v>
       </c>
-      <c r="B10">
+      <c r="B10" s="2">
         <v>25</v>
       </c>
-      <c r="C10">
+      <c r="C10" s="2">
         <v>55</v>
       </c>
-      <c r="D10">
+      <c r="D10" s="4">
         <v>25.5</v>
       </c>
-      <c r="E10">
+      <c r="E10" s="4">
         <v>47.5</v>
       </c>
-      <c r="F10">
+      <c r="F10" s="4">
         <v>17</v>
       </c>
-      <c r="G10">
+      <c r="G10" s="4">
         <v>31.66667</v>
       </c>
-      <c r="H10">
+      <c r="H10" s="4">
         <v>25.33333</v>
       </c>
-      <c r="I10">
+      <c r="I10" s="4">
         <v>50</v>
       </c>
-      <c r="J10">
+      <c r="J10" s="4">
         <v>16.88889</v>
       </c>
-      <c r="K10">
+      <c r="K10" s="4">
         <v>33.333329999999997</v>
       </c>
-      <c r="L10">
+      <c r="L10" s="5">
         <v>0.5</v>
       </c>
-      <c r="M10">
+      <c r="M10" s="5">
         <v>-7.5</v>
       </c>
-      <c r="N10">
+      <c r="N10" s="5">
         <v>-8</v>
       </c>
-      <c r="O10">
+      <c r="O10" s="5">
         <v>-23.33333</v>
       </c>
-      <c r="P10">
+      <c r="P10" s="5">
         <v>0.33333000000000002</v>
       </c>
-      <c r="Q10">
+      <c r="Q10" s="5">
         <v>-5</v>
       </c>
-      <c r="R10">
+      <c r="R10" s="5">
         <v>-8.1111000000000004</v>
       </c>
-      <c r="S10">
+      <c r="S10" s="5">
         <v>-21.66666</v>
       </c>
+      <c r="T10" s="6">
+        <f t="shared" si="1"/>
+        <v>0.5</v>
+      </c>
+      <c r="U10" s="6">
+        <f t="shared" si="0"/>
+        <v>7.5</v>
+      </c>
+      <c r="V10" s="6">
+        <f t="shared" si="0"/>
+        <v>8</v>
+      </c>
+      <c r="W10" s="6">
+        <f t="shared" si="0"/>
+        <v>23.33333</v>
+      </c>
+      <c r="X10" s="6">
+        <f t="shared" si="0"/>
+        <v>0.33333000000000002</v>
+      </c>
+      <c r="Y10" s="6">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
+      <c r="Z10" s="6">
+        <f t="shared" si="0"/>
+        <v>8.1111000000000004</v>
+      </c>
+      <c r="AA10" s="6">
+        <f t="shared" si="0"/>
+        <v>21.66666</v>
+      </c>
+      <c r="AB10" s="3">
+        <v>-0.02</v>
+      </c>
+      <c r="AC10" s="3">
+        <v>0.14599999999999999</v>
+      </c>
+      <c r="AD10" s="3">
+        <v>0.38100000000000001</v>
+      </c>
+      <c r="AE10" s="3">
+        <v>0.53800000000000003</v>
+      </c>
+      <c r="AF10" s="3">
+        <v>-1.2999999999999999E-2</v>
+      </c>
+      <c r="AG10" s="3">
+        <v>9.5000000000000001E-2</v>
+      </c>
+      <c r="AH10" s="3">
+        <v>0.38700000000000001</v>
+      </c>
+      <c r="AI10" s="3">
+        <v>0.49099999999999999</v>
+      </c>
+      <c r="AJ10" s="1">
+        <v>1.6E-2</v>
+      </c>
+      <c r="AK10" s="1">
+        <v>-0.16900000000000001</v>
+      </c>
+      <c r="AL10" s="1">
+        <v>-0.255</v>
+      </c>
+      <c r="AM10" s="1">
+        <v>-0.52600000000000002</v>
+      </c>
+      <c r="AN10" s="1">
+        <v>0.01</v>
+      </c>
+      <c r="AO10" s="1">
+        <v>-0.11</v>
+      </c>
+      <c r="AP10" s="1">
+        <v>-0.25900000000000001</v>
+      </c>
+      <c r="AQ10" s="1">
+        <v>-0.48899999999999999</v>
+      </c>
     </row>
-    <row r="11" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>10</v>
       </c>
-      <c r="B11">
+      <c r="B11" s="2">
         <v>30</v>
       </c>
-      <c r="C11">
+      <c r="C11" s="2">
         <v>35</v>
       </c>
-      <c r="D11">
+      <c r="D11" s="4">
         <v>30</v>
       </c>
-      <c r="E11">
+      <c r="E11" s="4">
         <v>40</v>
       </c>
-      <c r="F11">
+      <c r="F11" s="4">
         <v>20</v>
       </c>
-      <c r="G11">
+      <c r="G11" s="4">
         <v>26.66666</v>
       </c>
-      <c r="H11">
+      <c r="H11" s="4">
         <v>30</v>
       </c>
-      <c r="I11">
+      <c r="I11" s="4">
         <v>38.333329999999997</v>
       </c>
-      <c r="J11">
+      <c r="J11" s="4">
         <v>20</v>
       </c>
-      <c r="K11">
+      <c r="K11" s="4">
         <v>25.55555</v>
       </c>
-      <c r="L11">
-        <v>0</v>
-      </c>
-      <c r="M11">
+      <c r="L11" s="5">
+        <v>0</v>
+      </c>
+      <c r="M11" s="5">
         <v>5</v>
       </c>
-      <c r="N11">
+      <c r="N11" s="5">
         <v>-10</v>
       </c>
-      <c r="O11">
+      <c r="O11" s="5">
         <v>-8.3333300000000001</v>
       </c>
-      <c r="P11">
-        <v>0</v>
-      </c>
-      <c r="Q11">
+      <c r="P11" s="5">
+        <v>0</v>
+      </c>
+      <c r="Q11" s="5">
         <v>3.3333333000000001</v>
       </c>
-      <c r="R11">
+      <c r="R11" s="5">
         <v>-10</v>
       </c>
-      <c r="S11">
+      <c r="S11" s="5">
         <v>-9.4444440000000007</v>
+      </c>
+      <c r="T11" s="6">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="U11" s="6">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
+      <c r="V11" s="6">
+        <f t="shared" si="0"/>
+        <v>10</v>
+      </c>
+      <c r="W11" s="6">
+        <f t="shared" si="0"/>
+        <v>8.3333300000000001</v>
+      </c>
+      <c r="X11" s="6">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="Y11" s="6">
+        <f t="shared" si="0"/>
+        <v>3.3333333000000001</v>
+      </c>
+      <c r="Z11" s="6">
+        <f t="shared" si="0"/>
+        <v>10</v>
+      </c>
+      <c r="AA11" s="6">
+        <f t="shared" si="0"/>
+        <v>9.4444440000000007</v>
+      </c>
+      <c r="AB11" s="3">
+        <v>0</v>
+      </c>
+      <c r="AC11" s="3">
+        <v>-0.13300000000000001</v>
+      </c>
+      <c r="AD11" s="3">
+        <v>0.4</v>
+      </c>
+      <c r="AE11" s="3">
+        <v>0.27</v>
+      </c>
+      <c r="AF11" s="3">
+        <v>0</v>
+      </c>
+      <c r="AG11" s="3">
+        <v>-9.0999999999999998E-2</v>
+      </c>
+      <c r="AH11" s="3">
+        <v>0.4</v>
+      </c>
+      <c r="AI11" s="3">
+        <v>0.312</v>
+      </c>
+      <c r="AJ11" s="1">
+        <v>0</v>
+      </c>
+      <c r="AK11" s="1">
+        <v>0.183</v>
+      </c>
+      <c r="AL11" s="1">
+        <v>-0.26100000000000001</v>
+      </c>
+      <c r="AM11" s="1">
+        <v>-0.30499999999999999</v>
+      </c>
+      <c r="AN11" s="1">
+        <v>0</v>
+      </c>
+      <c r="AO11" s="1">
+        <v>0.12</v>
+      </c>
+      <c r="AP11" s="1">
+        <v>-0.26100000000000001</v>
+      </c>
+      <c r="AQ11" s="1">
+        <v>-0.34599999999999997</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="0" copies="0" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>